<commit_message>
fuel conif vs decid
</commit_message>
<xml_diff>
--- a/scenarios.xlsx
+++ b/scenarios.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\MEDMOD\SpatialModelsR\MEDSPREAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B88AAB5-C5EF-4C11-8C46-53BED4908E80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D27CF75-716B-444A-9067-7B4E481CEA40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9687B63A-F89B-47E3-AB36-04820FAA1C94}"/>
+    <workbookView xWindow="35385" yWindow="990" windowWidth="8850" windowHeight="4590" xr2:uid="{9687B63A-F89B-47E3-AB36-04820FAA1C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Obj4" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="25">
   <si>
     <t>scn.id</t>
   </si>
@@ -48,58 +49,67 @@
     <t>sr.opt</t>
   </si>
   <si>
+    <t>fuel.opt</t>
+  </si>
+  <si>
+    <t>facc</t>
+  </si>
+  <si>
+    <t>rpb</t>
+  </si>
+  <si>
+    <t>pb.upper.th</t>
+  </si>
+  <si>
+    <t>wslope</t>
+  </si>
+  <si>
+    <t>wwind</t>
+  </si>
+  <si>
+    <t>file.fire.ignis</t>
+  </si>
+  <si>
+    <t>file.sprd.weight</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
     <t>fuel</t>
   </si>
   <si>
-    <t>pb.upper.th</t>
-  </si>
-  <si>
-    <t>rpb</t>
-  </si>
-  <si>
-    <t>wslope</t>
-  </si>
-  <si>
-    <t>wwind</t>
-  </si>
-  <si>
-    <t>file.fire.ignis</t>
-  </si>
-  <si>
-    <t>obs</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>FireIgnitions</t>
   </si>
   <si>
+    <t>WeightSprdFactors</t>
+  </si>
+  <si>
     <t>pb=1-exp(-acc*fi)+U[-rp,rpb], fi=sr*fuel</t>
   </si>
   <si>
-    <t>B</t>
+    <t>GC0.1</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>GC0.1</t>
-  </si>
-  <si>
     <t>GC0.1, SH1</t>
   </si>
   <si>
-    <t>fuel.opt</t>
-  </si>
-  <si>
-    <t>facc</t>
-  </si>
-  <si>
-    <t>file.sprd.weight</t>
-  </si>
-  <si>
-    <t>WeightSprdFactors</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -123,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +152,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -155,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -177,6 +193,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,23 +512,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E19859F-333D-4C16-89F4-8572D04BF0E4}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="7.5546875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="10" width="8.77734375" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
@@ -528,34 +549,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -564,16 +585,16 @@
       </c>
       <c r="B2" s="3" t="str">
         <f>+_xlfn.CONCAT("Scn_pbEXPFI_wind",C2,"slope",D2,"fuel",E2,"_acc",F2,"_rpb",G2*10,"_up",H2*10,"_wDefault")</f>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb3_up8_wDefault</v>
+        <v>Scn_pbEXPFI_windAslopeAfuelC_acc2_rpb3_up8_wDefault</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4">
         <v>2</v>
@@ -587,16 +608,16 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -606,16 +627,16 @@
       </c>
       <c r="B3" s="3" t="str">
         <f>+_xlfn.CONCAT("Scn_pbEXPFI_wind",C3,"slope",D3,"fuel",E3,"_acc",F3,"_rpb",G3*10,"_up",H3*10,"_wDefault")</f>
-        <v>Scn_pbEXPFI_windAslopeAfuelC_acc2_rpb3_up8_wDefault</v>
+        <v>Scn_pbEXPFI_windAslopeAfuelD_acc2_rpb3_up8_wDefault</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -629,122 +650,122 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <f t="shared" ref="A4:A13" si="0">+A3+1</f>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f>+A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="str">
+      <c r="B4" s="3" t="str">
         <f>+_xlfn.CONCAT("Scn_pbEXPFI_wind",C4,"slope",D4,"fuel",E4,"_acc",F4,"_rpb",G4*10,"_up",H4*10,"_wDefault")</f>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb1_up8_wDefault</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="9">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="H4" s="9">
+        <v>Scn_pbEXPFI_windAslopeAfuelE_acc2_rpb3_up8_wDefault</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="4">
         <v>0.8</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="9" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f>+A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="str">
-        <f t="shared" ref="B5:B12" si="1">+_xlfn.CONCAT("Scn_pbEXPFI_wind",C5,"slope",D5,"fuel",E5,"_acc",F5,"_rpb",G5*10,"_up",H5*10,"_wDefault")</f>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb1_up8_wDefault</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="B5" s="3" t="str">
+        <f>+_xlfn.CONCAT("Scn_pbEXPFI_wind",C5,"slope",D5,"fuel",E5,"_acc",F5,"_rpb",G5*10,"_up",H5*10,"_wDefault")</f>
+        <v>Scn_pbEXPFI_windAslopeAfuelF_acc2_rpb3_up8_wDefault</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="9">
+      <c r="G5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H5" s="4">
         <v>0.8</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="9" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
-        <f t="shared" si="0"/>
+        <f>+A5+1</f>
         <v>5</v>
       </c>
       <c r="B6" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb1_up8_wDefault</v>
+        <f>+_xlfn.CONCAT("Scn_pbEXPFI_wind",C6,"slope",D6,"fuel",E6,"_acc",F6,"_rpb",G6*10,"_up",H6*10,"_wDefault")</f>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb1_up8_wDefault</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="9">
         <v>0.1</v>
@@ -755,41 +776,41 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
-        <f t="shared" si="0"/>
+        <f>+A6+1</f>
         <v>6</v>
       </c>
       <c r="B7" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb2_up8_wDefault</v>
+        <f t="shared" ref="B7:B14" si="0">+_xlfn.CONCAT("Scn_pbEXPFI_wind",C7,"slope",D7,"fuel",E7,"_acc",F7,"_rpb",G7*10,"_up",H7*10,"_wDefault")</f>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb1_up8_wDefault</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="9">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="9">
         <v>0.8</v>
@@ -797,41 +818,41 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
+        <f t="shared" ref="A7:A33" si="1">+A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb2_up8_wDefault</v>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb1_up8_wDefault</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="9">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H8" s="9">
         <v>0.8</v>
@@ -839,38 +860,38 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb2_up8_wDefault</v>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb2_up8_wDefault</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" s="9">
         <v>0.2</v>
@@ -881,41 +902,41 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb3_up8_wDefault</v>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb2_up8_wDefault</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="9">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H10" s="9">
         <v>0.8</v>
@@ -923,41 +944,41 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb3_up8_wDefault</v>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb2_up8_wDefault</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F11" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="9">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H11" s="9">
         <v>0.8</v>
@@ -965,38 +986,38 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb3_up8_wDefault</v>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb3_up8_wDefault</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F12" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G12" s="9">
         <v>0.3</v>
@@ -1007,61 +1028,918 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="B13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb3_up8_wDefault</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="9">
+        <v>2</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb3_up8_wDefault</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="9">
+        <v>3</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f>+_xlfn.CONCAT("Scn_pbEXPFI_wind",C15,"slope",D15,"fuel",E15,"_acc",F15,"_rpb",G15*10,"_up",H15*10,"_wDefault")</f>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb1_up10_wDefault</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="14">
+        <v>1</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="14">
+        <v>1</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f t="shared" ref="B16:B23" si="2">+_xlfn.CONCAT("Scn_pbEXPFI_wind",C16,"slope",D16,"fuel",E16,"_acc",F16,"_rpb",G16*10,"_up",H16*10,"_wDefault")</f>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb1_up10_wDefault</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="14">
+        <v>2</v>
+      </c>
+      <c r="G16" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N16" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb1_up10_wDefault</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="14">
+        <v>3</v>
+      </c>
+      <c r="G17" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="14">
+        <v>1</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb2_up10_wDefault</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="14">
+        <v>1</v>
+      </c>
+      <c r="G18" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb2_up10_wDefault</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="14">
+        <v>2</v>
+      </c>
+      <c r="G19" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="14">
+        <v>1</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb2_up10_wDefault</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="14">
+        <v>3</v>
+      </c>
+      <c r="G20" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="H20" s="14">
+        <v>1</v>
+      </c>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb3_up10_wDefault</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="14">
+        <v>1</v>
+      </c>
+      <c r="G21" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="H21" s="14">
+        <v>1</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="M12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="str">
-        <f t="shared" ref="B13" si="2">+_xlfn.CONCAT("Scn_pbEXPFI_wind",C13,"slope",D13, "fuel",E13, "_acc",F13, "_rpb",G13*10,"_up",H13*10,"_ws",I13*10,"_ww",10*J13)</f>
+      <c r="B22" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb3_up10_wDefault</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="14">
+        <v>2</v>
+      </c>
+      <c r="G22" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="H22" s="14">
+        <v>1</v>
+      </c>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb3_up10_wDefault</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="14">
+        <v>3</v>
+      </c>
+      <c r="G23" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="H23" s="14">
+        <v>1</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="13" t="str">
+        <f>+_xlfn.CONCAT("Scn_pbEXPFI_wind",C24,"slope",D24,"fuel",E24,"_acc",F24,"_rpb",G24*10,"_up",H24*10,"_wDefault")</f>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb1_up6_wDefault</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="14">
+        <v>1</v>
+      </c>
+      <c r="G24" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H24" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="13" t="str">
+        <f t="shared" ref="B25:B32" si="3">+_xlfn.CONCAT("Scn_pbEXPFI_wind",C25,"slope",D25,"fuel",E25,"_acc",F25,"_rpb",G25*10,"_up",H25*10,"_wDefault")</f>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb1_up6_wDefault</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="14">
+        <v>2</v>
+      </c>
+      <c r="G25" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H25" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N25" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb1_up6_wDefault</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="14">
+        <v>3</v>
+      </c>
+      <c r="G26" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H26" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb2_up6_wDefault</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="14">
+        <v>1</v>
+      </c>
+      <c r="G27" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="H27" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N27" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb2_up6_wDefault</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="14">
+        <v>2</v>
+      </c>
+      <c r="G28" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="H28" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N28" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb2_up6_wDefault</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="14">
+        <v>3</v>
+      </c>
+      <c r="G29" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="H29" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc1_rpb3_up6_wDefault</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="14">
+        <v>1</v>
+      </c>
+      <c r="G30" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="H30" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc2_rpb3_up6_wDefault</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="14">
+        <v>2</v>
+      </c>
+      <c r="G31" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="H31" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="13">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb3_up6_wDefault</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="14">
+        <v>3</v>
+      </c>
+      <c r="G32" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="H32" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N32" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="str">
+        <f t="shared" ref="B33" si="4">+_xlfn.CONCAT("Scn_pbEXPFI_wind",C33,"slope",D33, "fuel",E33, "_acc",F33, "_rpb",G33*10,"_up",H33*10,"_ws",I33*10,"_ww",10*J33)</f>
         <v>Scn_pbEXPFI_windAslopeAfuelB_acc3_rpb3_up8_ws0_ww0</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="11">
+      <c r="C33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="11">
         <v>3</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G33" s="11">
         <v>0.3</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H33" s="11">
         <v>0.8</v>
       </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="11" t="s">
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N33" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC90E6F-89AC-4A3D-828F-2B7D50492705}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C14708">
+    <sortCondition descending="1" ref="C1:C14708"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>